<commit_message>
add notebook with graph
</commit_message>
<xml_diff>
--- a/wip/unique_stock.xlsx
+++ b/wip/unique_stock.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -15931,6 +15931,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -16035,10 +16036,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.12"/>
@@ -24655,6 +24656,9 @@
       </c>
       <c r="B1017" s="0" t="s">
         <v>975</v>
+      </c>
+      <c r="C1017" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1018" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>